<commit_message>
initial Commit + Vin partial match tests
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="73">
   <si>
     <t>VIN</t>
   </si>
@@ -207,6 +207,42 @@
   </si>
   <si>
     <t>CA_MAKE_TEXT</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Arteon</t>
+  </si>
+  <si>
+    <t>Arteon SEL</t>
+  </si>
+  <si>
+    <t>Coupe</t>
+  </si>
+  <si>
+    <t>Sedan</t>
+  </si>
+  <si>
+    <t>8L V12</t>
+  </si>
+  <si>
+    <t>4WD</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>8MSRP17H&amp;V</t>
   </si>
 </sst>
 </file>
@@ -553,7 +589,7 @@
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,7 +1194,120 @@
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="3">
+        <v>88888</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="3">
+        <v>12</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>214</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" s="3">
+        <v>4</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="3">
+        <v>2</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>35</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>20000101</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Partial match case finished. Fix for add since member ship xpath
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -23,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Petrenko, Viktor (C)</author>
+  </authors>
+  <commentList>
+    <comment ref="AA6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Petrenko, Viktor (C):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+User for MSRP PAS-730</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="71">
   <si>
     <t>VIN</t>
   </si>
@@ -209,30 +243,12 @@
     <t>CA_MAKE_TEXT</t>
   </si>
   <si>
-    <t>Volkswagen</t>
-  </si>
-  <si>
-    <t>Arteon</t>
-  </si>
-  <si>
-    <t>Arteon SEL</t>
-  </si>
-  <si>
-    <t>Coupe</t>
-  </si>
-  <si>
-    <t>Sedan</t>
-  </si>
-  <si>
     <t>8L V12</t>
   </si>
   <si>
     <t>4WD</t>
   </si>
   <si>
-    <t>GC</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -243,13 +259,25 @@
   </si>
   <si>
     <t>8MSRP17H&amp;V</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN</t>
+  </si>
+  <si>
+    <t>GOLF</t>
+  </si>
+  <si>
+    <t>HATCHBACK 4 DOOR</t>
+  </si>
+  <si>
+    <t>RT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +299,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.4"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +329,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -298,11 +351,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -585,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,27 +1252,27 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="3">
-        <v>2017</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>62</v>
+        <v>2015</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H6" s="3">
         <v>88888</v>
@@ -1221,20 +1280,20 @@
       <c r="I6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>64</v>
+      <c r="J6" t="s">
+        <v>69</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O6" s="3">
         <v>12</v>
@@ -1246,7 +1305,7 @@
         <v>214</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="S6" s="3">
         <v>4</v>
@@ -1270,31 +1329,31 @@
         <v>37</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>35</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>44</v>
+        <v>70</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>33</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>43</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AD6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AG6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="AI6" s="3">
         <v>20000101</v>
@@ -1312,5 +1371,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PAS-730: CA choice covered
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -258,9 +258,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>8MSRP17H&amp;V</t>
-  </si>
-  <si>
     <t>VOLKSWAGEN</t>
   </si>
   <si>
@@ -271,13 +268,16 @@
   </si>
   <si>
     <t>RT</t>
+  </si>
+  <si>
+    <t>7MSRP15H&amp;V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,12 +300,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.4"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
@@ -319,7 +313,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,12 +323,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -351,17 +339,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -647,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,9 +1234,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>41</v>
@@ -1263,16 +1245,16 @@
         <v>2015</v>
       </c>
       <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
         <v>67</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="H6" s="3">
         <v>88888</v>
@@ -1281,13 +1263,13 @@
         <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
@@ -1329,12 +1311,12 @@
         <v>37</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA6" s="5">
+        <v>69</v>
+      </c>
+      <c r="AA6" s="3">
         <v>33</v>
       </c>
-      <c r="AB6" s="5">
+      <c r="AB6" s="3">
         <v>43</v>
       </c>
       <c r="AC6" s="3" t="s">
@@ -1355,16 +1337,16 @@
       <c r="AH6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AI6">
         <v>20000101</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AJ6" t="s">
         <v>38</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AK6" t="s">
         <v>38</v>
       </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AL6" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PAS-730: Small fixed for old test faced during execution. Changed dates for control tables to delete overlap.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -234,9 +234,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>CA_MAKE</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>4WD</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -271,6 +265,12 @@
   </si>
   <si>
     <t>7MSRP15H&amp;V</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,10 +781,10 @@
         <v>2005</v>
       </c>
       <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
         <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -862,16 +862,16 @@
         <v>38</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AI2">
         <v>20000101</v>
@@ -897,10 +897,10 @@
         <v>2005</v>
       </c>
       <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
         <v>59</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -978,16 +978,16 @@
         <v>38</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="AI3">
         <v>20000101</v>
@@ -1013,10 +1013,10 @@
         <v>2005</v>
       </c>
       <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
         <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
@@ -1129,10 +1129,10 @@
         <v>2005</v>
       </c>
       <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
         <v>59</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
@@ -1210,16 +1210,16 @@
         <v>38</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AG5" s="3" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="AI5">
         <v>20190101</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>41</v>
@@ -1245,16 +1245,16 @@
         <v>2015</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" s="3">
         <v>88888</v>
@@ -1263,19 +1263,19 @@
         <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O6" s="3">
         <v>12</v>
@@ -1287,7 +1287,7 @@
         <v>214</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S6" s="3">
         <v>4</v>
@@ -1311,7 +1311,7 @@
         <v>37</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA6" s="3">
         <v>33</v>
@@ -1326,16 +1326,16 @@
         <v>38</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="AI6">
         <v>20000101</v>

</xml_diff>

<commit_message>
PAS-535 PAS-2712, PAS-2714 fixes
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
   <si>
     <t>VIN</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -629,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,7 +1198,7 @@
         <v>37</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="AA5" s="3">
         <v>39</v>

</xml_diff>

<commit_message>
PAS-6576 Update "individual VIN retrieval" logic to use ENTRY DATE and VALID Made appropriate changes to the VIN Upload files Made some remarks in the tests
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
   <si>
     <t>VIN</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>invalidVin</t>
+  </si>
+  <si>
+    <t>SecondValid</t>
+  </si>
+  <si>
+    <t>ThirdValid</t>
   </si>
 </sst>
 </file>
@@ -632,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,6 +651,7 @@
     <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" customWidth="1"/>
     <col min="15" max="15" width="18.77734375" customWidth="1"/>
@@ -877,7 +887,7 @@
         <v>63</v>
       </c>
       <c r="AI2">
-        <v>20000101</v>
+        <v>20010101</v>
       </c>
       <c r="AJ2" t="s">
         <v>38</v>
@@ -906,7 +916,7 @@
         <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -1022,7 +1032,7 @@
         <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>28</v>
@@ -1138,7 +1148,7 @@
         <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
PAS-6576 fixed VIN upload files for choice and select products, changed BI symbols values from C to A (or vice-versa, I don't remember)
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -642,7 +642,7 @@
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,16 +875,16 @@
         <v>38</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AI2">
         <v>20010101</v>
@@ -1107,16 +1107,16 @@
         <v>38</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="AI4">
         <v>20150101</v>

</xml_diff>

<commit_message>
Fixes for CA VIN Refresh Tests: **Added the After suite line that will reset the DB back to default configurations **Changed VIN upload files so that the 'Make' will properly display and not blow up tests **Modified checks to no longer look for 'CA_MAKE', instead will look for 'Toyota' **Modified DB reset query to refer to correct MSRP Version **Did for Select and Choice products
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="76">
   <si>
     <t>VIN</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>ThirdValid</t>
+  </si>
+  <si>
+    <t>TOYOTA</t>
   </si>
 </sst>
 </file>
@@ -642,32 +645,32 @@
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
-    <col min="21" max="21" width="22.88671875" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
-    <col min="24" max="24" width="20.88671875" customWidth="1"/>
-    <col min="25" max="25" width="34.77734375" customWidth="1"/>
-    <col min="26" max="26" width="6.5546875" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" customWidth="1"/>
-    <col min="28" max="29" width="16.21875" customWidth="1"/>
-    <col min="35" max="35" width="15.109375" customWidth="1"/>
-    <col min="37" max="37" width="22.6640625" customWidth="1"/>
-    <col min="38" max="38" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="21" max="21" width="22.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="34.7109375" customWidth="1"/>
+    <col min="26" max="26" width="6.5703125" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="28" max="29" width="16.28515625" customWidth="1"/>
+    <col min="35" max="35" width="15.140625" customWidth="1"/>
+    <col min="37" max="37" width="22.7109375" customWidth="1"/>
+    <col min="38" max="38" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,7 +786,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -794,10 +797,10 @@
         <v>2005</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -899,7 +902,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Minor test suite tweaks
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
   <si>
     <t>VIN</t>
   </si>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t>ThirdValid</t>
-  </si>
-  <si>
-    <t>TOYOTA</t>
   </si>
 </sst>
 </file>
@@ -645,32 +642,32 @@
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="21" max="21" width="22.85546875" customWidth="1"/>
-    <col min="23" max="23" width="22.28515625" customWidth="1"/>
-    <col min="24" max="24" width="20.85546875" customWidth="1"/>
-    <col min="25" max="25" width="34.7109375" customWidth="1"/>
-    <col min="26" max="26" width="6.5703125" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="29" width="16.28515625" customWidth="1"/>
-    <col min="35" max="35" width="15.140625" customWidth="1"/>
-    <col min="37" max="37" width="22.7109375" customWidth="1"/>
-    <col min="38" max="38" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="15" max="15" width="18.77734375" customWidth="1"/>
+    <col min="21" max="21" width="22.88671875" customWidth="1"/>
+    <col min="23" max="23" width="22.21875" customWidth="1"/>
+    <col min="24" max="24" width="20.88671875" customWidth="1"/>
+    <col min="25" max="25" width="34.77734375" customWidth="1"/>
+    <col min="26" max="26" width="6.5546875" customWidth="1"/>
+    <col min="27" max="27" width="14.88671875" customWidth="1"/>
+    <col min="28" max="29" width="16.21875" customWidth="1"/>
+    <col min="35" max="35" width="15.109375" customWidth="1"/>
+    <col min="37" max="37" width="22.6640625" customWidth="1"/>
+    <col min="38" max="38" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +783,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -797,10 +794,10 @@
         <v>2005</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -902,7 +899,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1018,7 +1015,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1134,7 +1131,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1250,7 +1247,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Test suite updates 4/20
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_CHOICE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="76">
   <si>
     <t>VIN</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>ThirdValid</t>
+  </si>
+  <si>
+    <t>TOYOTA</t>
   </si>
 </sst>
 </file>
@@ -642,32 +645,32 @@
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
-    <col min="21" max="21" width="22.88671875" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
-    <col min="24" max="24" width="20.88671875" customWidth="1"/>
-    <col min="25" max="25" width="34.77734375" customWidth="1"/>
-    <col min="26" max="26" width="6.5546875" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" customWidth="1"/>
-    <col min="28" max="29" width="16.21875" customWidth="1"/>
-    <col min="35" max="35" width="15.109375" customWidth="1"/>
-    <col min="37" max="37" width="22.6640625" customWidth="1"/>
-    <col min="38" max="38" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="21" max="21" width="22.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="34.7109375" customWidth="1"/>
+    <col min="26" max="26" width="6.5703125" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="28" max="29" width="16.28515625" customWidth="1"/>
+    <col min="35" max="35" width="15.140625" customWidth="1"/>
+    <col min="37" max="37" width="22.7109375" customWidth="1"/>
+    <col min="38" max="38" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,7 +786,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -794,10 +797,10 @@
         <v>2005</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -899,7 +902,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>

</xml_diff>